<commit_message>
Fix rounding error in hydgn/SoHPCCbRIC
</commit_message>
<xml_diff>
--- a/InputData/hydgn/SoHPCCbRIC/Share of Hydrogen Production Capital Costs by Recipient ISIC Code.xlsx
+++ b/InputData/hydgn/SoHPCCbRIC/Share of Hydrogen Production Capital Costs by Recipient ISIC Code.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\hydgn\SoHPCCbRIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2D1DB3-56AD-420B-A58E-7967EE7EC440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954FA072-557B-4B1C-AD35-32F1A1902771}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="585" windowWidth="24090" windowHeight="16650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1224,7 +1224,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -1257,6 +1256,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2055,22 +2055,22 @@
       <c r="B33" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="54"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F34" s="54"/>
-      <c r="G34" s="54"/>
-      <c r="H34" s="54"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
     </row>
     <row r="35" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C35" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F35" s="54"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="54"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
     </row>
     <row r="36" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C36" s="3"/>
@@ -2085,22 +2085,22 @@
       <c r="C38" s="5">
         <v>50000</v>
       </c>
-      <c r="D38" s="55" t="s">
+      <c r="D38" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
-      <c r="H38" s="57"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="55"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="56"/>
     </row>
     <row r="39" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D39" s="58" t="s">
+      <c r="D39" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="E39" s="52"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="52"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
@@ -2109,11 +2109,11 @@
       <c r="C40" s="7">
         <v>2012</v>
       </c>
-      <c r="D40" s="59"/>
-      <c r="E40" s="60"/>
-      <c r="F40" s="60"/>
-      <c r="G40" s="60"/>
-      <c r="H40" s="61"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="59"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="59"/>
+      <c r="H40" s="60"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
@@ -2122,11 +2122,11 @@
       <c r="C41" s="8">
         <v>2010</v>
       </c>
-      <c r="D41" s="62"/>
-      <c r="E41" s="63"/>
-      <c r="F41" s="63"/>
-      <c r="G41" s="63"/>
-      <c r="H41" s="64"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="62"/>
+      <c r="F41" s="62"/>
+      <c r="G41" s="62"/>
+      <c r="H41" s="63"/>
     </row>
     <row r="42" spans="2:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
@@ -2135,13 +2135,13 @@
       <c r="C42" s="9">
         <v>0.94218268901813196</v>
       </c>
-      <c r="D42" s="62" t="s">
+      <c r="D42" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="E42" s="63"/>
-      <c r="F42" s="63"/>
-      <c r="G42" s="63"/>
-      <c r="H42" s="64"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="63"/>
       <c r="M42" t="s">
         <v>0</v>
       </c>
@@ -2156,13 +2156,13 @@
       <c r="C43" s="10">
         <v>1.100724186648488</v>
       </c>
-      <c r="D43" s="51" t="s">
+      <c r="D43" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="E43" s="52"/>
-      <c r="F43" s="52"/>
-      <c r="G43" s="52"/>
-      <c r="H43" s="53"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="51"/>
+      <c r="H43" s="52"/>
       <c r="M43" t="s">
         <v>1</v>
       </c>
@@ -2935,10 +2935,11 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="38" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="49" t="s">
         <v>132</v>
       </c>
       <c r="B1" t="s">
@@ -3057,151 +3058,151 @@
       <c r="A2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="49">
+      <c r="B2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,B1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="C2" s="49">
+      <c r="C2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,C1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="49">
+      <c r="D2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,D1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="E2" s="49">
+      <c r="E2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,E1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="F2" s="49">
+      <c r="F2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,F1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="G2" s="49">
+      <c r="G2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,G1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="H2" s="49">
+      <c r="H2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,H1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="I2" s="49">
+      <c r="I2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,I1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="J2" s="49">
+      <c r="J2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,J1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="K2" s="49">
+      <c r="K2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,K1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="L2" s="49">
+      <c r="L2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,L1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="M2" s="49">
+      <c r="M2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,M1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="N2" s="49">
+      <c r="N2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,N1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="O2" s="49">
+      <c r="O2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,O1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="P2" s="49">
+      <c r="P2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,P1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="Q2" s="49">
+      <c r="Q2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,Q1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="R2" s="49">
+      <c r="R2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,R1,Data!$J$47:$J$58)</f>
         <v>0.20535714285714285</v>
       </c>
-      <c r="S2" s="49">
+      <c r="S2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,S1,Data!$J$47:$J$58)</f>
         <v>0.66964285714285687</v>
       </c>
-      <c r="T2" s="49">
+      <c r="T2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,T1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="U2" s="49">
+      <c r="U2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,U1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="V2" s="49">
+      <c r="V2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,V1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="W2" s="49">
+      <c r="W2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,W1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="X2" s="49">
+      <c r="X2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,X1,Data!$J$47:$J$58)</f>
         <v>0.12499999999999986</v>
       </c>
-      <c r="Y2" s="49">
+      <c r="Y2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,Y1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="Z2" s="49">
+      <c r="Z2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,Z1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="AA2" s="49">
+      <c r="AA2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,AA1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="49">
+      <c r="AB2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,AB1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="AC2" s="49">
+      <c r="AC2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,AC1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="AD2" s="49">
+      <c r="AD2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,AD1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="AE2" s="49">
+      <c r="AE2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,AE1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="AF2" s="49">
+      <c r="AF2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,AF1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="AG2" s="49">
+      <c r="AG2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,AG1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="AH2" s="49">
+      <c r="AH2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,AH1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="AI2" s="49">
+      <c r="AI2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,AI1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="AJ2" s="49">
+      <c r="AJ2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,AJ1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="AK2" s="49">
+      <c r="AK2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,AK1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
-      <c r="AL2" s="49">
+      <c r="AL2" s="64">
         <f>SUMIF(Data!$I$47:$I$58,AL1,Data!$J$47:$J$58)</f>
         <v>0</v>
       </c>
@@ -3210,151 +3211,151 @@
       <c r="A3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="49">
+      <c r="B3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!B1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="C3" s="49">
+      <c r="C3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!C1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="D3" s="49">
+      <c r="D3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!D1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="E3" s="49">
+      <c r="E3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!E1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="F3" s="49">
+      <c r="F3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!F1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="G3" s="49">
+      <c r="G3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!G1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="H3" s="49">
+      <c r="H3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!H1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="49">
+      <c r="I3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!I1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="J3" s="49">
+      <c r="J3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!J1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="49">
+      <c r="K3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!K1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="L3" s="49">
+      <c r="L3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!L1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="M3" s="49">
+      <c r="M3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!M1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="N3" s="49">
+      <c r="N3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!N1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="O3" s="49">
+      <c r="O3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!O1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="P3" s="49">
+      <c r="P3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!P1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="49">
+      <c r="Q3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!Q1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="R3" s="49">
+      <c r="R3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!R1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="S3" s="49">
+      <c r="S3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!S1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0.41966165941316863</v>
       </c>
-      <c r="T3" s="49">
+      <c r="T3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!T1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="U3" s="49">
+      <c r="U3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!U1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="V3" s="49">
+      <c r="V3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!V1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="W3" s="49">
+      <c r="W3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!W1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="X3" s="49">
+      <c r="X3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!X1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0.41367167392016474</v>
       </c>
-      <c r="Y3" s="49">
+      <c r="Y3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!Y1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="Z3" s="49">
+      <c r="Z3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!Z1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="AA3" s="49">
+      <c r="AA3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!AA1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="AB3" s="49">
+      <c r="AB3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!AB1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="AC3" s="49">
+      <c r="AC3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!AC1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="AD3" s="49">
+      <c r="AD3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!AD1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="AE3" s="49">
+      <c r="AE3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!AE1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="AF3" s="49">
+      <c r="AF3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!AF1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="AG3" s="49">
+      <c r="AG3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!AG1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="AH3" s="49">
+      <c r="AH3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!AH1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="AI3" s="49">
+      <c r="AI3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!AI1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="AJ3" s="49">
+      <c r="AJ3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!AJ1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="AK3" s="49">
+      <c r="AK3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!AK1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
-      <c r="AL3" s="49">
+      <c r="AL3" s="64">
         <f>SUMIF(Data!$M$10:$M$21,SoHPCCbRIC!AL1,Data!$L$10:$L$21)/SUM(Data!$L$10:$L$21)</f>
         <v>0</v>
       </c>
@@ -3363,151 +3364,151 @@
       <c r="A4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="49">
+      <c r="B4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,B1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="C4" s="49">
+      <c r="C4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,C1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="D4" s="49">
+      <c r="D4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,D1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="E4" s="49">
+      <c r="E4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,E1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="49">
+      <c r="F4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,F1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="49">
+      <c r="G4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,G1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="49">
+      <c r="H4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,H1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="49">
+      <c r="I4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,I1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="J4" s="49">
+      <c r="J4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,J1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="49">
+      <c r="K4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,K1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="L4" s="49">
+      <c r="L4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,L1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="M4" s="49">
+      <c r="M4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,M1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="49">
+      <c r="N4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,N1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="O4" s="49">
+      <c r="O4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,O1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="P4" s="49">
+      <c r="P4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,P1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="49">
+      <c r="Q4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,Q1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="R4" s="49">
+      <c r="R4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,R1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="S4" s="49">
+      <c r="S4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,S1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0.55991337252195439</v>
       </c>
-      <c r="T4" s="49">
+      <c r="T4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,T1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="U4" s="49">
+      <c r="U4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,U1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="V4" s="49">
+      <c r="V4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,V1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="W4" s="49">
+      <c r="W4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,W1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="X4" s="49">
+      <c r="X4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,X1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0.34917537304552704</v>
       </c>
-      <c r="Y4" s="49">
+      <c r="Y4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,Y1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="Z4" s="49">
+      <c r="Z4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,Z1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="AA4" s="49">
+      <c r="AA4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,AA1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="AB4" s="49">
+      <c r="AB4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,AB1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="AC4" s="49">
+      <c r="AC4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,AC1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="AD4" s="49">
+      <c r="AD4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,AD1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="AE4" s="49">
+      <c r="AE4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,AE1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>9.0911254432518629E-2</v>
       </c>
-      <c r="AF4" s="49">
+      <c r="AF4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,AF1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="AG4" s="49">
+      <c r="AG4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,AG1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="AH4" s="49">
+      <c r="AH4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,AH1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="AI4" s="49">
+      <c r="AI4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,AI1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="AJ4" s="49">
+      <c r="AJ4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,AJ1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="AK4" s="49">
+      <c r="AK4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,AK1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
-      <c r="AL4" s="49">
+      <c r="AL4" s="64">
         <f>SUMIF(Data!$L$86:$L$95,AL1,Data!$K$86:$K$95)/SUM(Data!$K$86:$K$95)</f>
         <v>0</v>
       </c>
@@ -3516,151 +3517,151 @@
       <c r="A5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="49">
+      <c r="B5" s="64">
         <f>B4</f>
         <v>0</v>
       </c>
-      <c r="C5" s="49">
+      <c r="C5" s="64">
         <f t="shared" ref="C5:AL5" si="0">C4</f>
         <v>0</v>
       </c>
-      <c r="D5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="49">
+      <c r="D5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="64">
         <f t="shared" ref="L5" si="1">L4</f>
         <v>0</v>
       </c>
-      <c r="M5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S5" s="49">
+      <c r="M5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S5" s="64">
         <f t="shared" si="0"/>
         <v>0.55991337252195439</v>
       </c>
-      <c r="T5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="X5" s="49">
+      <c r="T5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X5" s="64">
         <f t="shared" si="0"/>
         <v>0.34917537304552704</v>
       </c>
-      <c r="Y5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Z5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AA5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AB5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AC5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AE5" s="49">
+      <c r="Y5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AC5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE5" s="64">
         <f t="shared" si="0"/>
         <v>9.0911254432518629E-2</v>
       </c>
-      <c r="AF5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AG5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AH5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AK5" s="49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AL5" s="49">
+      <c r="AF5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AG5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AI5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AK5" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AL5" s="64">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3669,151 +3670,151 @@
       <c r="A6" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="49">
+      <c r="B6" s="64">
         <f>B4</f>
         <v>0</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="64">
         <f t="shared" ref="C6:AL6" si="2">C4</f>
         <v>0</v>
       </c>
-      <c r="D6" s="49">
+      <c r="D6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E6" s="49">
+      <c r="E6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F6" s="49">
+      <c r="F6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G6" s="49">
+      <c r="G6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H6" s="49">
+      <c r="H6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I6" s="49">
+      <c r="I6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J6" s="49">
+      <c r="J6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K6" s="49">
+      <c r="K6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L6" s="49">
+      <c r="L6" s="64">
         <f t="shared" ref="L6" si="3">L4</f>
         <v>0</v>
       </c>
-      <c r="M6" s="49">
+      <c r="M6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N6" s="49">
+      <c r="N6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O6" s="49">
+      <c r="O6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P6" s="49">
+      <c r="P6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q6" s="49">
+      <c r="Q6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R6" s="49">
+      <c r="R6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S6" s="49">
+      <c r="S6" s="64">
         <f t="shared" si="2"/>
         <v>0.55991337252195439</v>
       </c>
-      <c r="T6" s="49">
+      <c r="T6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U6" s="49">
+      <c r="U6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="V6" s="49">
+      <c r="V6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W6" s="49">
+      <c r="W6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X6" s="49">
+      <c r="X6" s="64">
         <f t="shared" si="2"/>
         <v>0.34917537304552704</v>
       </c>
-      <c r="Y6" s="49">
+      <c r="Y6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Z6" s="49">
+      <c r="Z6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA6" s="49">
+      <c r="AA6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB6" s="49">
+      <c r="AB6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC6" s="49">
+      <c r="AC6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AD6" s="49">
+      <c r="AD6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AE6" s="49">
+      <c r="AE6" s="64">
         <f t="shared" si="2"/>
         <v>9.0911254432518629E-2</v>
       </c>
-      <c r="AF6" s="49">
+      <c r="AF6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AG6" s="49">
+      <c r="AG6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AH6" s="49">
+      <c r="AH6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AI6" s="49">
+      <c r="AI6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AJ6" s="49">
+      <c r="AJ6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AK6" s="49">
+      <c r="AK6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AL6" s="49">
+      <c r="AL6" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>

</xml_diff>